<commit_message>
Ver 0.2.08: Added ADS Meta
</commit_message>
<xml_diff>
--- a/Development/Data/PackageData/PackageDataFredaP21.xlsx
+++ b/Development/Data/PackageData/PackageDataFredaP21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsFredaP21\Development\Data\PackageData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE868B9D-7031-4BAC-BE4B-DC3E5F194D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0E6F31-6A20-40C5-ADD2-0D2752B38D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="23040" windowHeight="12120" tabRatio="724" activeTab="1" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="23040" windowHeight="12120" tabRatio="724" activeTab="2" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta.Tables" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="562">
   <si>
     <t>D</t>
   </si>
@@ -569,9 +569,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Physician</t>
-  </si>
-  <si>
     <t>Admission by Physician</t>
   </si>
   <si>
@@ -584,27 +581,18 @@
     <t>Notfall</t>
   </si>
   <si>
-    <t>Transfer-long</t>
-  </si>
-  <si>
     <t>Transfer from Other Hospital after Stay of more than 24 hours</t>
   </si>
   <si>
     <t>Verlegung mit Behandlungsdauer im verlegenden Krankenhaus länger als 24 Stunden</t>
   </si>
   <si>
-    <t>Transfer-short</t>
-  </si>
-  <si>
     <t>Transfer from Other Hospital after Stay of less than 24 hours</t>
   </si>
   <si>
     <t>Verlegung mit Behandlungsdauer im verlegenden Krankenhaus bis zu 24 Stunden</t>
   </si>
   <si>
-    <t>PostRehabilitation</t>
-  </si>
-  <si>
     <t>Admission after Stay in Rehabilitation</t>
   </si>
   <si>
@@ -612,9 +600,6 @@
   </si>
   <si>
     <t>Z</t>
-  </si>
-  <si>
-    <t>Dentist</t>
   </si>
   <si>
     <t>Admission by Dentist</t>
@@ -5602,7 +5587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BF945-9186-40D3-A998-0B845CD0DDFC}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
     </sheetView>
@@ -7131,7 +7116,7 @@
         <v>157</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="H34" s="3" t="s">
         <v>28</v>
@@ -7223,7 +7208,7 @@
         <v>159</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>28</v>
@@ -7269,7 +7254,7 @@
         <v>160</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>28</v>
@@ -7788,11 +7773,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF1C1D3-3AE0-4822-BECE-5F11FDFA805B}">
   <dimension ref="A1:N1295"/>
   <sheetViews>
-    <sheetView zoomScale="79" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -8059,13 +8044,13 @@
         <v>26</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="I8" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8092,13 +8077,13 @@
         <v>14</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8125,13 +8110,13 @@
         <v>17</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="I10" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8158,13 +8143,13 @@
         <v>13</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>181</v>
+        <v>13</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8191,13 +8176,13 @@
         <v>9</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>184</v>
+        <v>9</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8221,16 +8206,16 @@
         <v>Nominal</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8254,16 +8239,16 @@
         <v>Nominal</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8290,13 +8275,13 @@
         <v>7</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>194</v>
+        <v>7</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8374,16 +8359,16 @@
         <v>Nominal</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8407,16 +8392,16 @@
         <v>Nominal</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8440,16 +8425,16 @@
         <v>Nominal</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8473,16 +8458,16 @@
         <v>Nominal</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8506,16 +8491,16 @@
         <v>Nominal</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8539,16 +8524,16 @@
         <v>Nominal</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8572,16 +8557,16 @@
         <v>Nominal</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8605,16 +8590,16 @@
         <v>Nominal</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8638,16 +8623,16 @@
         <v>Nominal</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8671,16 +8656,16 @@
         <v>Nominal</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8704,16 +8689,16 @@
         <v>Nominal</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8737,16 +8722,16 @@
         <v>Nominal</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8770,16 +8755,16 @@
         <v>Nominal</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8803,16 +8788,16 @@
         <v>Nominal</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8836,16 +8821,16 @@
         <v>Nominal</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8869,16 +8854,16 @@
         <v>Nominal</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8902,16 +8887,16 @@
         <v>Nominal</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8935,16 +8920,16 @@
         <v>Nominal</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -8968,16 +8953,16 @@
         <v>Nominal</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9001,16 +8986,16 @@
         <v>Nominal</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9034,16 +9019,16 @@
         <v>Nominal</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9067,16 +9052,16 @@
         <v>Nominal</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9100,16 +9085,16 @@
         <v>Nominal</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9133,16 +9118,16 @@
         <v>Nominal</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9166,16 +9151,16 @@
         <v>Nominal</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9199,16 +9184,16 @@
         <v>Nominal</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9232,16 +9217,16 @@
         <v>Nominal</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9265,16 +9250,16 @@
         <v>Nominal</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9298,16 +9283,16 @@
         <v>Nominal</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9331,16 +9316,16 @@
         <v>Nominal</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9364,16 +9349,16 @@
         <v>Nominal</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9397,16 +9382,16 @@
         <v>Nominal</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9430,16 +9415,16 @@
         <v>Nominal</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9463,16 +9448,16 @@
         <v>Nominal</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9496,16 +9481,16 @@
         <v>Nominal</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9529,16 +9514,16 @@
         <v>Nominal</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="I53" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9562,16 +9547,16 @@
         <v>Nominal</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9595,16 +9580,16 @@
         <v>Nominal</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9628,16 +9613,16 @@
         <v>Nominal</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="I56" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9661,16 +9646,16 @@
         <v>Nominal</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="I57" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9694,16 +9679,16 @@
         <v>Nominal</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9727,16 +9712,16 @@
         <v>Nominal</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9760,16 +9745,16 @@
         <v>Nominal</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9793,16 +9778,16 @@
         <v>Nominal</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9826,16 +9811,16 @@
         <v>Nominal</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9859,16 +9844,16 @@
         <v>Nominal</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9892,16 +9877,16 @@
         <v>Nominal</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9925,16 +9910,16 @@
         <v>Nominal</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9958,16 +9943,16 @@
         <v>Nominal</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -9991,16 +9976,16 @@
         <v>Nominal</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10024,16 +10009,16 @@
         <v>Nominal</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10057,16 +10042,16 @@
         <v>Nominal</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10090,16 +10075,16 @@
         <v>Nominal</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10123,16 +10108,16 @@
         <v>Nominal</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="I71" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10156,16 +10141,16 @@
         <v>Nominal</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10189,16 +10174,16 @@
         <v>Nominal</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10222,16 +10207,16 @@
         <v>Nominal</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10255,16 +10240,16 @@
         <v>Nominal</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10288,16 +10273,16 @@
         <v>Nominal</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10321,16 +10306,16 @@
         <v>Nominal</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10354,16 +10339,16 @@
         <v>Nominal</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I78" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10387,16 +10372,16 @@
         <v>Nominal</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="I79" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10420,16 +10405,16 @@
         <v>Nominal</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="81" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10453,16 +10438,16 @@
         <v>Nominal</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10486,16 +10471,16 @@
         <v>Nominal</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="83" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10519,16 +10504,16 @@
         <v>Nominal</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10552,16 +10537,16 @@
         <v>Nominal</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10585,16 +10570,16 @@
         <v>Nominal</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10618,16 +10603,16 @@
         <v>Nominal</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="87" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10651,16 +10636,16 @@
         <v>Nominal</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10684,16 +10669,16 @@
         <v>Nominal</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10717,16 +10702,16 @@
         <v>Nominal</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10750,16 +10735,16 @@
         <v>Nominal</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10783,16 +10768,16 @@
         <v>Nominal</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10816,16 +10801,16 @@
         <v>Nominal</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10849,16 +10834,16 @@
         <v>Nominal</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10882,16 +10867,16 @@
         <v>Nominal</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="95" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10915,16 +10900,16 @@
         <v>Nominal</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10948,16 +10933,16 @@
         <v>Nominal</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -10981,16 +10966,16 @@
         <v>Nominal</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11014,16 +10999,16 @@
         <v>Nominal</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11047,16 +11032,16 @@
         <v>Nominal</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11080,16 +11065,16 @@
         <v>Nominal</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11113,16 +11098,16 @@
         <v>Nominal</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="I101" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11146,16 +11131,16 @@
         <v>Nominal</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11179,16 +11164,16 @@
         <v>Nominal</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11212,16 +11197,16 @@
         <v>Nominal</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11245,16 +11230,16 @@
         <v>Nominal</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11278,16 +11263,16 @@
         <v>Nominal</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11311,16 +11296,16 @@
         <v>Nominal</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11344,16 +11329,16 @@
         <v>Nominal</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="109" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11377,16 +11362,16 @@
         <v>Nominal</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="110" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11410,16 +11395,16 @@
         <v>Nominal</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11443,16 +11428,16 @@
         <v>Nominal</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
     <row r="112" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11476,16 +11461,16 @@
         <v>Nominal</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
     </row>
     <row r="113" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11509,16 +11494,16 @@
         <v>Nominal</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="114" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11542,16 +11527,16 @@
         <v>Nominal</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="I114" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="115" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11575,16 +11560,16 @@
         <v>Nominal</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="116" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11608,16 +11593,16 @@
         <v>Nominal</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="I116" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="117" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11641,16 +11626,16 @@
         <v>Nominal</v>
       </c>
       <c r="F117" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
     </row>
     <row r="118" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11674,16 +11659,16 @@
         <v>Nominal</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="119" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11707,16 +11692,16 @@
         <v>Nominal</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="120" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11740,16 +11725,16 @@
         <v>Nominal</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="121" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11773,16 +11758,16 @@
         <v>Nominal</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="122" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11806,16 +11791,16 @@
         <v>Nominal</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
     </row>
     <row r="123" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11839,16 +11824,16 @@
         <v>Nominal</v>
       </c>
       <c r="F123" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
     </row>
     <row r="124" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11872,16 +11857,16 @@
         <v>Nominal</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="125" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11905,16 +11890,16 @@
         <v>Nominal</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="126" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11938,16 +11923,16 @@
         <v>Nominal</v>
       </c>
       <c r="F126" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="127" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -11971,16 +11956,16 @@
         <v>Nominal</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="H127" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="128" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12004,16 +11989,16 @@
         <v>Nominal</v>
       </c>
       <c r="F128" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="H128" s="1" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="I128" s="1" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
     </row>
     <row r="129" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12037,16 +12022,16 @@
         <v>Nominal</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="H129" s="1" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
     </row>
     <row r="130" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12070,16 +12055,16 @@
         <v>Nominal</v>
       </c>
       <c r="F130" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="H130" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="I130" s="1" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
     </row>
     <row r="131" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12103,16 +12088,16 @@
         <v>Nominal</v>
       </c>
       <c r="F131" s="3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="H131" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
     </row>
     <row r="132" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12136,16 +12121,16 @@
         <v>Nominal</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
     </row>
     <row r="133" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12169,16 +12154,16 @@
         <v>Nominal</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="134" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12202,16 +12187,16 @@
         <v>Nominal</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="H134" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
     </row>
     <row r="135" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12235,16 +12220,16 @@
         <v>Nominal</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="H135" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="136" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12268,16 +12253,16 @@
         <v>Nominal</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="H136" s="1" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="I136" s="1" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12301,16 +12286,16 @@
         <v>Nominal</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="H137" s="1" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="138" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12334,16 +12319,16 @@
         <v>Nominal</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="H138" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12367,16 +12352,16 @@
         <v>Nominal</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="H139" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12400,16 +12385,16 @@
         <v>Nominal</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="H140" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I140" s="1" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12433,16 +12418,16 @@
         <v>Nominal</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="H141" s="1" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12466,16 +12451,16 @@
         <v>Nominal</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="H142" s="1" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12499,16 +12484,16 @@
         <v>Nominal</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="H143" s="1" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
     </row>
     <row r="144" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12532,16 +12517,16 @@
         <v>Nominal</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="H144" s="1" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12565,16 +12550,16 @@
         <v>Nominal</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="H145" s="1" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="146" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12598,16 +12583,16 @@
         <v>Nominal</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="H146" s="1" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
     </row>
     <row r="147" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12631,16 +12616,16 @@
         <v>Nominal</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="H147" s="1" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="I147" s="1" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="148" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12664,16 +12649,16 @@
         <v>Nominal</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="H148" s="1" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="I148" s="1" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="149" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12697,16 +12682,16 @@
         <v>Nominal</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="G149" s="3" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="H149" s="1" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="I149" s="1" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
     </row>
     <row r="150" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12730,16 +12715,16 @@
         <v>Nominal</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="G150" s="3" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="H150" s="1" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="I150" s="1" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="151" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12763,16 +12748,16 @@
         <v>Nominal</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="G151" s="3" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="H151" s="1" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="I151" s="1" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="152" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12796,16 +12781,16 @@
         <v>Nominal</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="H152" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="I152" s="1" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="153" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12829,16 +12814,16 @@
         <v>Nominal</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="H153" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="I153" s="1" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="154" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12862,16 +12847,16 @@
         <v>Nominal</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="H154" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="I154" s="1" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
     </row>
     <row r="155" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12895,16 +12880,16 @@
         <v>Nominal</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="G155" s="3" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="H155" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="I155" s="1" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="156" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12928,16 +12913,16 @@
         <v>Nominal</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="H156" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="I156" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="157" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12961,16 +12946,16 @@
         <v>Nominal</v>
       </c>
       <c r="F157" s="3" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="H157" s="1" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="I157" s="1" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
     </row>
     <row r="158" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -12994,16 +12979,16 @@
         <v>Nominal</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="G158" s="3" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="H158" s="1" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="I158" s="1" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
     </row>
     <row r="159" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13027,16 +13012,16 @@
         <v>Nominal</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="H159" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="I159" s="1" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
     </row>
     <row r="160" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13060,16 +13045,16 @@
         <v>Nominal</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="H160" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="I160" s="1" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="161" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13093,16 +13078,16 @@
         <v>Nominal</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="H161" s="1" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="I161" s="1" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="162" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13126,16 +13111,16 @@
         <v>Nominal</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="H162" s="1" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="I162" s="1" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="163" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13159,16 +13144,16 @@
         <v>Nominal</v>
       </c>
       <c r="F163" s="3" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="H163" s="1" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="I163" s="1" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
     </row>
     <row r="164" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13192,16 +13177,16 @@
         <v>Nominal</v>
       </c>
       <c r="F164" s="3" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="H164" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="I164" s="1" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
     </row>
     <row r="165" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13225,16 +13210,16 @@
         <v>Nominal</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="H165" s="1" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="I165" s="1" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="166" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13258,16 +13243,16 @@
         <v>Nominal</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="H166" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="I166" s="1" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="167" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13291,16 +13276,16 @@
         <v>Nominal</v>
       </c>
       <c r="F167" s="3" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="H167" s="1" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="I167" s="1" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="168" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13324,16 +13309,16 @@
         <v>Nominal</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="H168" s="1" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="I168" s="1" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="169" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13357,16 +13342,16 @@
         <v>Nominal</v>
       </c>
       <c r="F169" s="3" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="G169" s="3" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="H169" s="1" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="I169" s="1" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="170" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13390,16 +13375,16 @@
         <v>Nominal</v>
       </c>
       <c r="F170" s="3" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="G170" s="3" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="H170" s="1" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="I170" s="1" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="171" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13423,16 +13408,16 @@
         <v>Nominal</v>
       </c>
       <c r="F171" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="H171" s="1" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="I171" s="1" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="172" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13456,16 +13441,16 @@
         <v>Nominal</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="H172" s="1" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="I172" s="1" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="173" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13489,16 +13474,16 @@
         <v>Nominal</v>
       </c>
       <c r="F173" s="3" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="H173" s="1" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="I173" s="1" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="174" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13522,16 +13507,16 @@
         <v>Nominal</v>
       </c>
       <c r="F174" s="3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="G174" s="3" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="I174" s="1" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="175" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13555,16 +13540,16 @@
         <v>Nominal</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="G175" s="3" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="H175" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="176" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13588,16 +13573,16 @@
         <v>Nominal</v>
       </c>
       <c r="F176" s="3" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="H176" s="1" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="177" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13621,16 +13606,16 @@
         <v>Nominal</v>
       </c>
       <c r="F177" s="3" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="H177" s="1" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="178" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13654,16 +13639,16 @@
         <v>Nominal</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="H178" s="1" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="179" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13687,16 +13672,16 @@
         <v>Nominal</v>
       </c>
       <c r="F179" s="3" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="H179" s="1" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="180" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13720,16 +13705,16 @@
         <v>Nominal</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="H180" s="1" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="181" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13753,16 +13738,16 @@
         <v>Nominal</v>
       </c>
       <c r="F181" s="3" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="H181" s="1" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="182" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13786,16 +13771,16 @@
         <v>Nominal</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="H182" s="1" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="183" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13819,16 +13804,16 @@
         <v>Nominal</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="H183" s="1" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="I183" s="1" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
     </row>
     <row r="184" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13852,16 +13837,16 @@
         <v>Nominal</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="H184" s="1" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="185" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13885,16 +13870,16 @@
         <v>Nominal</v>
       </c>
       <c r="F185" s="3" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="H185" s="1" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
     </row>
     <row r="186" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13918,16 +13903,16 @@
         <v>Nominal</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="G186" s="3" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="H186" s="1" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
     </row>
     <row r="187" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13951,16 +13936,16 @@
         <v>Nominal</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="G187" s="3" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="H187" s="1" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
     </row>
     <row r="188" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -13984,16 +13969,16 @@
         <v>Nominal</v>
       </c>
       <c r="F188" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="H188" s="1" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
     </row>
     <row r="189" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14017,16 +14002,16 @@
         <v>Nominal</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="H189" s="1" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="I189" s="1" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
     </row>
     <row r="190" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14050,16 +14035,16 @@
         <v>Nominal</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="H190" s="1" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="I190" s="1" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
     </row>
     <row r="191" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14083,16 +14068,16 @@
         <v>Nominal</v>
       </c>
       <c r="F191" s="3" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="H191" s="1" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="I191" s="1" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
     </row>
     <row r="192" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14116,16 +14101,16 @@
         <v>Nominal</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="H192" s="1" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
       <c r="I192" s="1" t="s">
-        <v>545</v>
+        <v>540</v>
       </c>
     </row>
     <row r="193" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14149,16 +14134,16 @@
         <v>Nominal</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="H193" s="1" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="I193" s="1" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
     </row>
     <row r="194" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14182,16 +14167,16 @@
         <v>Nominal</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="H194" s="1" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="I194" s="1" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
     </row>
     <row r="195" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14215,16 +14200,16 @@
         <v>Nominal</v>
       </c>
       <c r="F195" s="3" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="H195" s="1" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="I195" s="1" t="s">
-        <v>551</v>
+        <v>546</v>
       </c>
     </row>
     <row r="196" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14248,16 +14233,16 @@
         <v>Nominal</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
       <c r="H196" s="1" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
       <c r="I196" s="1" t="s">
-        <v>553</v>
+        <v>548</v>
       </c>
     </row>
     <row r="197" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14281,16 +14266,16 @@
         <v>Nominal</v>
       </c>
       <c r="F197" s="3" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="G197" s="3" t="s">
-        <v>554</v>
+        <v>549</v>
       </c>
       <c r="H197" s="1" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
       <c r="I197" s="1" t="s">
-        <v>555</v>
+        <v>550</v>
       </c>
     </row>
     <row r="198" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14314,16 +14299,16 @@
         <v>Nominal</v>
       </c>
       <c r="F198" s="3" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="G198" s="3" t="s">
-        <v>556</v>
+        <v>551</v>
       </c>
       <c r="H198" s="1" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
       <c r="I198" s="1" t="s">
-        <v>557</v>
+        <v>552</v>
       </c>
     </row>
     <row r="199" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14347,16 +14332,16 @@
         <v>Nominal</v>
       </c>
       <c r="F199" s="3" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="G199" s="3" t="s">
-        <v>558</v>
+        <v>553</v>
       </c>
       <c r="H199" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
       <c r="I199" s="1" t="s">
-        <v>559</v>
+        <v>554</v>
       </c>
     </row>
     <row r="200" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14436,16 +14421,16 @@
         <v>Nominal</v>
       </c>
       <c r="F202" s="3" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="G202" s="3" t="s">
-        <v>560</v>
+        <v>555</v>
       </c>
       <c r="H202" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
       <c r="I202" s="1" t="s">
-        <v>561</v>
+        <v>556</v>
       </c>
     </row>
     <row r="203" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
@@ -14469,16 +14454,16 @@
         <v>Nominal</v>
       </c>
       <c r="F203" s="3" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="G203" s="3" t="s">
-        <v>562</v>
+        <v>557</v>
       </c>
       <c r="H203" s="1" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
       <c r="I203" s="1" t="s">
-        <v>563</v>
+        <v>558</v>
       </c>
     </row>
     <row r="204" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ver 0.2.09: Improved and generalized PrepareRawDataDS() (moved to dsFreda)
</commit_message>
<xml_diff>
--- a/Development/Data/PackageData/PackageDataFredaP21.xlsx
+++ b/Development/Data/PackageData/PackageDataFredaP21.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Basti\ARBEIT Lokal\dsFredaP21\Development\Data\PackageData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0E6F31-6A20-40C5-ADD2-0D2752B38D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{039C759B-C100-4231-B92B-0F6F2B8C6A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="23040" windowHeight="12120" tabRatio="724" activeTab="2" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="724" firstSheet="4" activeTab="8" xr2:uid="{035133D3-9E9F-4CDB-BCDC-A149BB1E9383}"/>
   </bookViews>
   <sheets>
     <sheet name="Meta.Tables" sheetId="11" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="565">
   <si>
     <t>D</t>
   </si>
@@ -1734,6 +1734,15 @@
   </si>
   <si>
     <t>LocalizationSecondaryICD10Code</t>
+  </si>
+  <si>
+    <t>str_to_lower(.X)</t>
+  </si>
+  <si>
+    <t>str_sub(.X, end = 2)</t>
+  </si>
+  <si>
+    <t>lubridate::parse_date_time(.X, orders = c('YmdHM', 'Ymd'))</t>
   </si>
 </sst>
 </file>
@@ -5587,8 +5596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD8BF945-9186-40D3-A998-0B845CD0DDFC}">
   <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
@@ -7773,7 +7782,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF1C1D3-3AE0-4822-BECE-5F11FDFA805B}">
   <dimension ref="A1:N1295"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
+    <sheetView zoomScale="79" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -26713,13 +26722,13 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46793C28-9A39-4A22-8D26-DFC8E119DCF7}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E35" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D40" sqref="D40"/>
+      <selection pane="bottomRight" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="25.2" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -26791,6 +26800,139 @@
         <v>39</v>
       </c>
     </row>
+    <row r="4" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="24">
+        <v>3</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f>VLOOKUP(B4,Meta.Features!$B:$G,$C$1,FALSE)</f>
+        <v>Case</v>
+      </c>
+      <c r="D4" s="31" t="str">
+        <f>VLOOKUP(B4,Meta.Features!$B:$G,$D$1,FALSE)</f>
+        <v>Sex</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="24">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="str">
+        <f>VLOOKUP(B5,Meta.Features!$B:$G,$C$1,FALSE)</f>
+        <v>Case</v>
+      </c>
+      <c r="D5" s="31" t="str">
+        <f>VLOOKUP(B5,Meta.Features!$B:$G,$D$1,FALSE)</f>
+        <v>AdmissionDate</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="24">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8" t="str">
+        <f>VLOOKUP(B6,Meta.Features!$B:$G,$C$1,FALSE)</f>
+        <v>Case</v>
+      </c>
+      <c r="D6" s="31" t="str">
+        <f>VLOOKUP(B6,Meta.Features!$B:$G,$D$1,FALSE)</f>
+        <v>DischargeDate</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="24">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8" t="str">
+        <f>VLOOKUP(B7,Meta.Features!$B:$G,$C$1,FALSE)</f>
+        <v>Case</v>
+      </c>
+      <c r="D7" s="31" t="str">
+        <f>VLOOKUP(B7,Meta.Features!$B:$G,$D$1,FALSE)</f>
+        <v>DischargeReasonCode</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="24">
+        <v>23</v>
+      </c>
+      <c r="C8" s="8" t="str">
+        <f>VLOOKUP(B8,Meta.Features!$B:$G,$C$1,FALSE)</f>
+        <v>Department</v>
+      </c>
+      <c r="D8" s="31" t="str">
+        <f>VLOOKUP(B8,Meta.Features!$B:$G,$D$1,FALSE)</f>
+        <v>DepartmentAdmissionDate</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="24">
+        <v>24</v>
+      </c>
+      <c r="C9" s="8" t="str">
+        <f>VLOOKUP(B9,Meta.Features!$B:$G,$C$1,FALSE)</f>
+        <v>Department</v>
+      </c>
+      <c r="D9" s="31" t="str">
+        <f>VLOOKUP(B9,Meta.Features!$B:$G,$D$1,FALSE)</f>
+        <v>DepartmentDischargeDate</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="24">
+        <v>43</v>
+      </c>
+      <c r="C10" s="8" t="str">
+        <f>VLOOKUP(B10,Meta.Features!$B:$G,$C$1,FALSE)</f>
+        <v>Procedure</v>
+      </c>
+      <c r="D10" s="31" t="str">
+        <f>VLOOKUP(B10,Meta.Features!$B:$G,$D$1,FALSE)</f>
+        <v>OPSDate</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>564</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>